<commit_message>
checkouts based on scenes
</commit_message>
<xml_diff>
--- a/Projects/MARSUAE_SAND/Tests/Data/test_case_1.xlsx
+++ b/Projects/MARSUAE_SAND/Tests/Data/test_case_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,8 +14,8 @@
     <sheet name="stitch_groups" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$29</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$127</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
@@ -33,16 +33,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$N$29</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$N$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$N$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$N$18</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="81">
   <si>
     <t xml:space="preserve">probe_match_fk</t>
   </si>
@@ -546,27 +548,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:127"/>
+  <dimension ref="1:129"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H119" activeCellId="0" sqref="H119"/>
+      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4773,8 +4774,74 @@
         <v>1</v>
       </c>
     </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>1101</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H128" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I128" s="0" t="n">
+        <f aca="false">VLOOKUP(H128, all_products!$A$2:$B$40, 2, 0)</f>
+        <v>20</v>
+      </c>
+      <c r="J128" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>1102</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G129" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H129" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I129" s="0" t="n">
+        <f aca="false">VLOOKUP(H129, all_products!$A$2:$B$40, 2, 0)</f>
+        <v>20</v>
+      </c>
+      <c r="J129" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J52"/>
+  <autoFilter ref="A1:J127"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4793,25 +4860,24 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2755102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5538,33 +5604,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S54"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O47" activeCellId="0" sqref="O47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.7142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6020408163265"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.8214285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.7448979591837"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9495,8 +9559,81 @@
         <v>13</v>
       </c>
     </row>
+    <row r="55" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="B55" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C55" s="10" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$201,matches!$B$2:$B$201,$A55,matches!$H$2:$H$201,$B55)</f>
+        <v>2</v>
+      </c>
+      <c r="D55" s="10" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$201,matches!$B$2:$B$201,$A55,matches!$H$2:$H$201,$B55, matches!$F$2:$F$201, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="E55" s="10" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$201,matches!$B$2:$B$201,$A55,matches!$H$2:$H$201,$B55)</f>
+        <v>40</v>
+      </c>
+      <c r="F55" s="10" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$201,matches!$B$2:$B$201,$A55,matches!$H$2:$H$201,$B55, matches!$F$2:$F$201, 1)</f>
+        <v>40</v>
+      </c>
+      <c r="G55" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J55" s="10" t="str">
+        <f aca="false">VLOOKUP(B55,all_products!$A$2:$C$40, 3, 0)</f>
+        <v>Product 4</v>
+      </c>
+      <c r="K55" s="10" t="str">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$G$40, 4, 0)</f>
+        <v>Chocolate</v>
+      </c>
+      <c r="L55" s="10" t="n">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$G$40, 5, 0)</f>
+        <v>6</v>
+      </c>
+      <c r="M55" s="10" t="n">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$G$40, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="N55" s="10" t="str">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$G$40, 7, 0)</f>
+        <v>Non-Mars</v>
+      </c>
+      <c r="O55" s="10" t="n">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$L$40, 8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P55" s="10" t="n">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$L$40, 9, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q55" s="10" t="n">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$L$40, 10, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R55" s="10" t="n">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$L$40, 11, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="S55" s="10" t="n">
+        <f aca="false">VLOOKUP($B55, all_products!$A$2:$L$40, 12, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N29"/>
+  <autoFilter ref="A1:N14"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -9513,16 +9650,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B128" activeCellId="0" sqref="B128"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B130" activeCellId="0" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10538,6 +10674,22 @@
         <v>1009</v>
       </c>
       <c r="B127" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>1101</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>1102</v>
+      </c>
+      <c r="B129" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>